<commit_message>
fix: add functional annotation of protein for yli
</commit_message>
<xml_diff>
--- a/data/Results sample_Data 20210406.xlsx
+++ b/data/Results sample_Data 20210406.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xluhon/Documents/GitHub/Yli_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D524A207-45FB-A64F-AF9B-D63E12F0FD21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928AA82D-5B46-174B-AE20-C5E36C684F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="26880" windowHeight="15080" activeTab="2" xr2:uid="{B9F56D9D-CEEC-E54C-A0C7-3282913CF77D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15080" activeTab="3" xr2:uid="{B9F56D9D-CEEC-E54C-A0C7-3282913CF77D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Samples" sheetId="1" r:id="rId1"/>
     <sheet name="Calculation" sheetId="3" r:id="rId2"/>
     <sheet name="Final" sheetId="4" r:id="rId3"/>
+    <sheet name="simple" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -208,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="112">
   <si>
     <t>Sample number</t>
   </si>
@@ -532,6 +533,75 @@
   <si>
     <t>co2和dcw影响 carbon balance</t>
   </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>W29∆ku70::cas9</t>
+  </si>
+  <si>
+    <t>W29∆ku70::cas9∆mhy1∆ARE1∆LRO1∆DGA1∆DGA2, lntC3: Tefp-AtCAD-Pex20p, GPDp-AtMTT-lip2t</t>
+  </si>
+  <si>
+    <t>RQ</t>
+  </si>
+  <si>
+    <t>qP mmol gCDW-1 h-1</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>mhy1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C2H2 finger domain transcription factor sebA</t>
+  </si>
+  <si>
+    <t>∆ARE1</t>
+  </si>
+  <si>
+    <t>∆LRO1</t>
+  </si>
+  <si>
+    <t>∆DGA1</t>
+  </si>
+  <si>
+    <t>∆DGA2</t>
+  </si>
+  <si>
+    <t>YALI0_F06578g</t>
+  </si>
+  <si>
+    <t>FUNCTION: Sterol O-acyltransferase that catalyzes the formation of stery esters. {ECO:0000256|ARBA:ARBA00023568}.</t>
+  </si>
+  <si>
+    <t>YALI0_E16797g</t>
+  </si>
+  <si>
+    <t>YALI0_E32769g</t>
+  </si>
+  <si>
+    <t>YALI0_D07986g</t>
+  </si>
+  <si>
+    <t>phospholipid:diacylglycerol acyltransferase</t>
+  </si>
+  <si>
+    <t>Diacylglycerol O-acyltransferase</t>
+  </si>
+  <si>
+    <t>O-acyltransferase</t>
+  </si>
 </sst>
 </file>
 
@@ -544,7 +614,7 @@
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -616,6 +686,19 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -718,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -863,15 +946,36 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6863,14 +6967,14 @@
         <f t="shared" ref="Z49:Z56" si="18">100*((W49+Y49)/(6*X49))</f>
         <v>90.136675102840996</v>
       </c>
-      <c r="AA49" s="88" t="s">
+      <c r="AA49" s="89" t="s">
         <v>49</v>
       </c>
-      <c r="AB49" s="88"/>
-      <c r="AC49" s="88"/>
-      <c r="AD49" s="88"/>
-      <c r="AE49" s="88"/>
-      <c r="AF49" s="88"/>
+      <c r="AB49" s="89"/>
+      <c r="AC49" s="89"/>
+      <c r="AD49" s="89"/>
+      <c r="AE49" s="89"/>
+      <c r="AF49" s="89"/>
       <c r="AG49">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -7011,12 +7115,12 @@
         <f t="shared" si="18"/>
         <v>82.11697356806188</v>
       </c>
-      <c r="AA50" s="88"/>
-      <c r="AB50" s="88"/>
-      <c r="AC50" s="88"/>
-      <c r="AD50" s="88"/>
-      <c r="AE50" s="88"/>
-      <c r="AF50" s="88"/>
+      <c r="AA50" s="89"/>
+      <c r="AB50" s="89"/>
+      <c r="AC50" s="89"/>
+      <c r="AD50" s="89"/>
+      <c r="AE50" s="89"/>
+      <c r="AF50" s="89"/>
       <c r="AG50">
         <v>1.2699999999999999E-2</v>
       </c>
@@ -7157,12 +7261,12 @@
         <f t="shared" si="18"/>
         <v>65.985058756677134</v>
       </c>
-      <c r="AA51" s="88"/>
-      <c r="AB51" s="88"/>
-      <c r="AC51" s="88"/>
-      <c r="AD51" s="88"/>
-      <c r="AE51" s="88"/>
-      <c r="AF51" s="88"/>
+      <c r="AA51" s="89"/>
+      <c r="AB51" s="89"/>
+      <c r="AC51" s="89"/>
+      <c r="AD51" s="89"/>
+      <c r="AE51" s="89"/>
+      <c r="AF51" s="89"/>
       <c r="AG51">
         <v>1.5100000000000001E-2</v>
       </c>
@@ -7301,12 +7405,12 @@
         <f t="shared" si="18"/>
         <v>83.414139628896095</v>
       </c>
-      <c r="AA52" s="88"/>
-      <c r="AB52" s="88"/>
-      <c r="AC52" s="88"/>
-      <c r="AD52" s="88"/>
-      <c r="AE52" s="88"/>
-      <c r="AF52" s="88"/>
+      <c r="AA52" s="89"/>
+      <c r="AB52" s="89"/>
+      <c r="AC52" s="89"/>
+      <c r="AD52" s="89"/>
+      <c r="AE52" s="89"/>
+      <c r="AF52" s="89"/>
       <c r="AG52">
         <v>1.72E-2</v>
       </c>
@@ -7442,12 +7546,12 @@
         <f t="shared" si="18"/>
         <v>82.807755793856231</v>
       </c>
-      <c r="AA53" s="88"/>
-      <c r="AB53" s="88"/>
-      <c r="AC53" s="88"/>
-      <c r="AD53" s="88"/>
-      <c r="AE53" s="88"/>
-      <c r="AF53" s="88"/>
+      <c r="AA53" s="89"/>
+      <c r="AB53" s="89"/>
+      <c r="AC53" s="89"/>
+      <c r="AD53" s="89"/>
+      <c r="AE53" s="89"/>
+      <c r="AF53" s="89"/>
       <c r="AG53">
         <v>2.3999999999999998E-3</v>
       </c>
@@ -15860,8 +15964,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A6DD82-743E-4531-A6C7-AFFA05AD9981}">
   <dimension ref="A1:AS17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15900,47 +16004,47 @@
       <c r="E1" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="90" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
-      <c r="M1" s="89"/>
-      <c r="N1" s="89"/>
-      <c r="O1" s="89"/>
-      <c r="P1" s="89"/>
-      <c r="Q1" s="89"/>
-      <c r="R1" s="89"/>
-      <c r="S1" s="89"/>
-      <c r="T1" s="89"/>
-      <c r="U1" s="89"/>
-      <c r="V1" s="89"/>
-      <c r="W1" s="89"/>
-      <c r="X1" s="89"/>
-      <c r="Y1" s="89"/>
-      <c r="Z1" s="89"/>
-      <c r="AA1" s="89"/>
-      <c r="AB1" s="89"/>
-      <c r="AC1" s="89"/>
-      <c r="AD1" s="89"/>
-      <c r="AE1" s="89"/>
-      <c r="AF1" s="89"/>
-      <c r="AG1" s="89"/>
-      <c r="AH1" s="89"/>
-      <c r="AI1" s="89"/>
-      <c r="AJ1" s="89"/>
-      <c r="AK1" s="89"/>
-      <c r="AL1" s="89"/>
-      <c r="AM1" s="89"/>
-      <c r="AN1" s="89"/>
-      <c r="AO1" s="89"/>
-      <c r="AP1" s="89"/>
-      <c r="AQ1" s="89"/>
-      <c r="AR1" s="89"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="90"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="90"/>
+      <c r="AL1" s="90"/>
+      <c r="AM1" s="90"/>
+      <c r="AN1" s="90"/>
+      <c r="AO1" s="90"/>
+      <c r="AP1" s="90"/>
+      <c r="AQ1" s="90"/>
+      <c r="AR1" s="90"/>
     </row>
     <row r="2" spans="1:45" s="56" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="59"/>
@@ -15976,7 +16080,7 @@
       <c r="N2" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="O2" s="90" t="s">
+      <c r="O2" s="88" t="s">
         <v>82</v>
       </c>
       <c r="P2" s="60" t="s">
@@ -17410,4 +17514,665 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7964DA19-5AD6-F443-A696-F959E4FB8966}">
+  <dimension ref="A1:AK13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A13" sqref="A9:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="8" style="8" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="80" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="28"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="58" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="90"/>
+      <c r="K1" s="90"/>
+      <c r="L1" s="90"/>
+      <c r="M1" s="90"/>
+      <c r="N1" s="90"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="90"/>
+      <c r="R1" s="90"/>
+      <c r="S1" s="90"/>
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="90"/>
+      <c r="X1" s="90"/>
+      <c r="Y1" s="90"/>
+      <c r="Z1" s="90"/>
+      <c r="AA1" s="90"/>
+      <c r="AB1" s="90"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="90"/>
+      <c r="AJ1" s="90"/>
+    </row>
+    <row r="2" spans="1:37" s="91" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="96"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="92" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="94" t="s">
+        <v>82</v>
+      </c>
+      <c r="H2" s="93" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="J2" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="93" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="93" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="93" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" s="93" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="93" t="s">
+        <v>96</v>
+      </c>
+      <c r="R2" s="93" t="s">
+        <v>77</v>
+      </c>
+      <c r="S2" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="92" t="s">
+        <v>60</v>
+      </c>
+      <c r="U2" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="92" t="s">
+        <v>24</v>
+      </c>
+      <c r="W2" s="92" t="s">
+        <v>25</v>
+      </c>
+      <c r="X2" s="92" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="92" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="92" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA2" s="92" t="s">
+        <v>28</v>
+      </c>
+      <c r="AB2" s="92" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" s="92" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD2" s="92" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE2" s="92" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF2" s="92" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG2" s="95" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH2" s="92" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI2" s="92" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ2" s="93" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="93"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3">
+        <v>0.28511388888888889</v>
+      </c>
+      <c r="F3">
+        <v>0.10274943310657597</v>
+      </c>
+      <c r="G3">
+        <v>2.3173276402759639</v>
+      </c>
+      <c r="H3">
+        <v>2.0611190344509009</v>
+      </c>
+      <c r="I3">
+        <f>H3/G3</f>
+        <v>0.88943790192976258</v>
+      </c>
+      <c r="J3">
+        <v>1.0435269370550675</v>
+      </c>
+      <c r="K3">
+        <v>7.7298574585497697E-4</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1.1918442079072571E-2</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>105.48094963478324</v>
+      </c>
+      <c r="S3">
+        <v>105.95673808436203</v>
+      </c>
+      <c r="T3" s="98">
+        <v>6.0286637702861946E-2</v>
+      </c>
+      <c r="U3">
+        <v>40.77687256813757</v>
+      </c>
+      <c r="V3">
+        <v>18.579755229238994</v>
+      </c>
+      <c r="W3">
+        <v>13.460994977967525</v>
+      </c>
+      <c r="X3">
+        <v>143.98991887665829</v>
+      </c>
+      <c r="Y3">
+        <v>72.019286205336186</v>
+      </c>
+      <c r="Z3">
+        <v>20.681266666666669</v>
+      </c>
+      <c r="AA3">
+        <v>3.4333333333333334E-3</v>
+      </c>
+      <c r="AB3">
+        <v>0</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>1.3166666666666667E-2</v>
+      </c>
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>0</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>25.0565</v>
+      </c>
+      <c r="AI3">
+        <v>4.375233333333334</v>
+      </c>
+      <c r="AJ3">
+        <v>167.08888888888887</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4">
+        <v>0.28438472222222222</v>
+      </c>
+      <c r="F4">
+        <v>0.10428743961352656</v>
+      </c>
+      <c r="G4" s="97">
+        <v>6.3868296243536635</v>
+      </c>
+      <c r="H4">
+        <v>2.2999059683422316</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I6" si="0">H4/G4</f>
+        <v>0.36010134974830776</v>
+      </c>
+      <c r="J4">
+        <v>1.3387433065091772</v>
+      </c>
+      <c r="K4">
+        <v>9.0474542442535476E-4</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0.12623135764988455</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>85.169728942079473</v>
+      </c>
+      <c r="S4">
+        <v>88.413855089759281</v>
+      </c>
+      <c r="T4" s="98">
+        <v>7.3966534094040193E-2</v>
+      </c>
+      <c r="U4">
+        <v>37.628733816742233</v>
+      </c>
+      <c r="V4">
+        <v>16.692397380749796</v>
+      </c>
+      <c r="W4">
+        <v>15.685381570146426</v>
+      </c>
+      <c r="X4">
+        <v>154.57209211767258</v>
+      </c>
+      <c r="Y4">
+        <v>65.470656307741351</v>
+      </c>
+      <c r="Z4">
+        <v>20.762133333333335</v>
+      </c>
+      <c r="AA4">
+        <v>3.2999999999999995E-3</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0.10856666666666666</v>
+      </c>
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
+        <v>0</v>
+      </c>
+      <c r="AG4">
+        <v>0</v>
+      </c>
+      <c r="AH4">
+        <v>25.305599999999998</v>
+      </c>
+      <c r="AI4">
+        <v>4.5434666666666663</v>
+      </c>
+      <c r="AJ4">
+        <v>201.42222222222219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="B5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5">
+        <v>0.19837222222222226</v>
+      </c>
+      <c r="F5">
+        <v>0.10419682057220052</v>
+      </c>
+      <c r="G5">
+        <v>4.819766280324977</v>
+      </c>
+      <c r="H5">
+        <v>3.1347595349761295</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0.65039658619396079</v>
+      </c>
+      <c r="J5">
+        <v>1.5012495723958532</v>
+      </c>
+      <c r="K5">
+        <v>5.1819918847651062E-3</v>
+      </c>
+      <c r="L5">
+        <v>1.3552921774277001E-2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1.500818884433223E-2</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>2.8332356039131417E-4</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>85.222596099932971</v>
+      </c>
+      <c r="S5">
+        <v>86.37003866174814</v>
+      </c>
+      <c r="T5" s="99">
+        <v>1.7679907819335386E-2</v>
+      </c>
+      <c r="U5">
+        <v>11.772205385678005</v>
+      </c>
+      <c r="V5">
+        <v>3.7081288185505694</v>
+      </c>
+      <c r="W5">
+        <v>1.8534297006513094</v>
+      </c>
+      <c r="X5">
+        <v>9.6410651668880902</v>
+      </c>
+      <c r="Y5">
+        <v>27.779632410850876</v>
+      </c>
+      <c r="Z5">
+        <v>21.496933333333335</v>
+      </c>
+      <c r="AA5">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="AB5">
+        <v>1.77E-2</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>1.0333333333333333E-2</v>
+      </c>
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AH5">
+        <v>25.514500000000002</v>
+      </c>
+      <c r="AI5">
+        <v>4.0175666666666681</v>
+      </c>
+      <c r="AJ5">
+        <v>238.58333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="B6" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6">
+        <v>0.16973888888888888</v>
+      </c>
+      <c r="F6">
+        <v>0.10419682057220052</v>
+      </c>
+      <c r="G6">
+        <v>2.7201165239439442</v>
+      </c>
+      <c r="H6">
+        <v>2.9325555218636379</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>1.0780992270182876</v>
+      </c>
+      <c r="J6">
+        <v>1.1464436653584047</v>
+      </c>
+      <c r="K6">
+        <v>3.1193551097403404E-3</v>
+      </c>
+      <c r="L6">
+        <v>8.6831247203256745E-3</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1.444908855651305E-2</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1.151509140274018E-2</v>
+      </c>
+      <c r="Q6">
+        <v>0.11770471404381526</v>
+      </c>
+      <c r="R6">
+        <v>108.89286960541926</v>
+      </c>
+      <c r="S6">
+        <v>119.26931310425171</v>
+      </c>
+      <c r="T6">
+        <v>1.7596708664456145E-2</v>
+      </c>
+      <c r="U6">
+        <v>10.411336911180776</v>
+      </c>
+      <c r="V6">
+        <v>1.8362213232096887</v>
+      </c>
+      <c r="W6">
+        <v>1.8021466167123201</v>
+      </c>
+      <c r="X6">
+        <v>8.7039799081834275</v>
+      </c>
+      <c r="Y6">
+        <v>29.316752910283125</v>
+      </c>
+      <c r="Z6">
+        <v>22.428100000000001</v>
+      </c>
+      <c r="AA6">
+        <v>8.4999999999999989E-3</v>
+      </c>
+      <c r="AB6">
+        <v>1.0833333333333334E-2</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>1.9233333333333335E-2</v>
+      </c>
+      <c r="AG6">
+        <v>0.19696666666666665</v>
+      </c>
+      <c r="AH6">
+        <v>25.364899999999995</v>
+      </c>
+      <c r="AI6">
+        <v>2.9367999999999994</v>
+      </c>
+      <c r="AJ6">
+        <v>251.7777777777778</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:AJ1"/>
+  </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix: update the script
</commit_message>
<xml_diff>
--- a/data/Results sample_Data 20210406.xlsx
+++ b/data/Results sample_Data 20210406.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xluhon/Documents/GitHub/Yli_GEMs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928AA82D-5B46-174B-AE20-C5E36C684F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597B8584-EEAF-6D45-8D97-18D6D312836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="15080" activeTab="3" xr2:uid="{B9F56D9D-CEEC-E54C-A0C7-3282913CF77D}"/>
+    <workbookView xWindow="1440" yWindow="1140" windowWidth="26880" windowHeight="15080" activeTab="3" xr2:uid="{B9F56D9D-CEEC-E54C-A0C7-3282913CF77D}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Samples" sheetId="1" r:id="rId1"/>
@@ -549,9 +549,6 @@
     <t>W29∆ku70::cas9</t>
   </si>
   <si>
-    <t>W29∆ku70::cas9∆mhy1∆ARE1∆LRO1∆DGA1∆DGA2, lntC3: Tefp-AtCAD-Pex20p, GPDp-AtMTT-lip2t</t>
-  </si>
-  <si>
     <t>RQ</t>
   </si>
   <si>
@@ -602,6 +599,47 @@
   <si>
     <t>O-acyltransferase</t>
   </si>
+  <si>
+    <r>
+      <t>W29∆ku70::cas9∆mhy1∆ARE1∆LRO1∆DGA1∆DGA2, lntC3: Tefp-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AtCAD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-Pex20p, GPDp-</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AtMTT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-lip2t</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -614,7 +652,7 @@
     <numFmt numFmtId="167" formatCode="0.000000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -701,6 +739,11 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="15">
@@ -949,12 +992,6 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -976,6 +1013,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6967,14 +7010,14 @@
         <f t="shared" ref="Z49:Z56" si="18">100*((W49+Y49)/(6*X49))</f>
         <v>90.136675102840996</v>
       </c>
-      <c r="AA49" s="89" t="s">
+      <c r="AA49" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="AB49" s="89"/>
-      <c r="AC49" s="89"/>
-      <c r="AD49" s="89"/>
-      <c r="AE49" s="89"/>
-      <c r="AF49" s="89"/>
+      <c r="AB49" s="98"/>
+      <c r="AC49" s="98"/>
+      <c r="AD49" s="98"/>
+      <c r="AE49" s="98"/>
+      <c r="AF49" s="98"/>
       <c r="AG49">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -7115,12 +7158,12 @@
         <f t="shared" si="18"/>
         <v>82.11697356806188</v>
       </c>
-      <c r="AA50" s="89"/>
-      <c r="AB50" s="89"/>
-      <c r="AC50" s="89"/>
-      <c r="AD50" s="89"/>
-      <c r="AE50" s="89"/>
-      <c r="AF50" s="89"/>
+      <c r="AA50" s="98"/>
+      <c r="AB50" s="98"/>
+      <c r="AC50" s="98"/>
+      <c r="AD50" s="98"/>
+      <c r="AE50" s="98"/>
+      <c r="AF50" s="98"/>
       <c r="AG50">
         <v>1.2699999999999999E-2</v>
       </c>
@@ -7261,12 +7304,12 @@
         <f t="shared" si="18"/>
         <v>65.985058756677134</v>
       </c>
-      <c r="AA51" s="89"/>
-      <c r="AB51" s="89"/>
-      <c r="AC51" s="89"/>
-      <c r="AD51" s="89"/>
-      <c r="AE51" s="89"/>
-      <c r="AF51" s="89"/>
+      <c r="AA51" s="98"/>
+      <c r="AB51" s="98"/>
+      <c r="AC51" s="98"/>
+      <c r="AD51" s="98"/>
+      <c r="AE51" s="98"/>
+      <c r="AF51" s="98"/>
       <c r="AG51">
         <v>1.5100000000000001E-2</v>
       </c>
@@ -7405,12 +7448,12 @@
         <f t="shared" si="18"/>
         <v>83.414139628896095</v>
       </c>
-      <c r="AA52" s="89"/>
-      <c r="AB52" s="89"/>
-      <c r="AC52" s="89"/>
-      <c r="AD52" s="89"/>
-      <c r="AE52" s="89"/>
-      <c r="AF52" s="89"/>
+      <c r="AA52" s="98"/>
+      <c r="AB52" s="98"/>
+      <c r="AC52" s="98"/>
+      <c r="AD52" s="98"/>
+      <c r="AE52" s="98"/>
+      <c r="AF52" s="98"/>
       <c r="AG52">
         <v>1.72E-2</v>
       </c>
@@ -7546,12 +7589,12 @@
         <f t="shared" si="18"/>
         <v>82.807755793856231</v>
       </c>
-      <c r="AA53" s="89"/>
-      <c r="AB53" s="89"/>
-      <c r="AC53" s="89"/>
-      <c r="AD53" s="89"/>
-      <c r="AE53" s="89"/>
-      <c r="AF53" s="89"/>
+      <c r="AA53" s="98"/>
+      <c r="AB53" s="98"/>
+      <c r="AC53" s="98"/>
+      <c r="AD53" s="98"/>
+      <c r="AE53" s="98"/>
+      <c r="AF53" s="98"/>
       <c r="AG53">
         <v>2.3999999999999998E-3</v>
       </c>
@@ -15964,8 +16007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A6DD82-743E-4531-A6C7-AFFA05AD9981}">
   <dimension ref="A1:AS17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16004,47 +16047,47 @@
       <c r="E1" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="90"/>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="90"/>
-      <c r="AD1" s="90"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="90"/>
-      <c r="AJ1" s="90"/>
-      <c r="AK1" s="90"/>
-      <c r="AL1" s="90"/>
-      <c r="AM1" s="90"/>
-      <c r="AN1" s="90"/>
-      <c r="AO1" s="90"/>
-      <c r="AP1" s="90"/>
-      <c r="AQ1" s="90"/>
-      <c r="AR1" s="90"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AJ1" s="99"/>
+      <c r="AK1" s="99"/>
+      <c r="AL1" s="99"/>
+      <c r="AM1" s="99"/>
+      <c r="AN1" s="99"/>
+      <c r="AO1" s="99"/>
+      <c r="AP1" s="99"/>
+      <c r="AQ1" s="99"/>
+      <c r="AR1" s="99"/>
     </row>
     <row r="2" spans="1:45" s="56" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="59"/>
@@ -17520,8 +17563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7964DA19-5AD6-F443-A696-F959E4FB8966}">
   <dimension ref="A1:AK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A13" sqref="A9:XFD13"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17539,141 +17582,141 @@
       <c r="E1" s="58" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="90" t="s">
+      <c r="F1" s="99" t="s">
         <v>61</v>
       </c>
-      <c r="G1" s="90"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
-      <c r="Z1" s="90"/>
-      <c r="AA1" s="90"/>
-      <c r="AB1" s="90"/>
-      <c r="AC1" s="90"/>
-      <c r="AD1" s="90"/>
-      <c r="AE1" s="90"/>
-      <c r="AF1" s="90"/>
-      <c r="AG1" s="90"/>
-      <c r="AH1" s="90"/>
-      <c r="AI1" s="90"/>
-      <c r="AJ1" s="90"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="99"/>
+      <c r="M1" s="99"/>
+      <c r="N1" s="99"/>
+      <c r="O1" s="99"/>
+      <c r="P1" s="99"/>
+      <c r="Q1" s="99"/>
+      <c r="R1" s="99"/>
+      <c r="S1" s="99"/>
+      <c r="T1" s="99"/>
+      <c r="U1" s="99"/>
+      <c r="V1" s="99"/>
+      <c r="W1" s="99"/>
+      <c r="X1" s="99"/>
+      <c r="Y1" s="99"/>
+      <c r="Z1" s="99"/>
+      <c r="AA1" s="99"/>
+      <c r="AB1" s="99"/>
+      <c r="AC1" s="99"/>
+      <c r="AD1" s="99"/>
+      <c r="AE1" s="99"/>
+      <c r="AF1" s="99"/>
+      <c r="AG1" s="99"/>
+      <c r="AH1" s="99"/>
+      <c r="AI1" s="99"/>
+      <c r="AJ1" s="99"/>
     </row>
-    <row r="2" spans="1:37" s="91" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="96"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92" t="s">
+    <row r="2" spans="1:37" s="89" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="94"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90" t="s">
         <v>63</v>
       </c>
-      <c r="F2" s="92" t="s">
+      <c r="F2" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="94" t="s">
+      <c r="G2" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="H2" s="93" t="s">
+      <c r="H2" s="91" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="93" t="s">
+      <c r="I2" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="J2" s="91" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="91" t="s">
+        <v>69</v>
+      </c>
+      <c r="L2" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="91" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="91" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="91" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2" s="91" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q2" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="93" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="93" t="s">
-        <v>69</v>
-      </c>
-      <c r="L2" s="93" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" s="93" t="s">
-        <v>71</v>
-      </c>
-      <c r="N2" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="O2" s="93" t="s">
-        <v>73</v>
-      </c>
-      <c r="P2" s="93" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q2" s="93" t="s">
-        <v>96</v>
-      </c>
-      <c r="R2" s="93" t="s">
+      <c r="R2" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="S2" s="93" t="s">
+      <c r="S2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="T2" s="92" t="s">
+      <c r="T2" s="90" t="s">
         <v>60</v>
       </c>
-      <c r="U2" s="92" t="s">
+      <c r="U2" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="V2" s="92" t="s">
+      <c r="V2" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="92" t="s">
+      <c r="W2" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="92" t="s">
+      <c r="X2" s="90" t="s">
         <v>26</v>
       </c>
-      <c r="Y2" s="92" t="s">
+      <c r="Y2" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="Z2" s="92" t="s">
+      <c r="Z2" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="92" t="s">
+      <c r="AA2" s="90" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="92" t="s">
+      <c r="AB2" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="92" t="s">
+      <c r="AC2" s="90" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="92" t="s">
+      <c r="AD2" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="92" t="s">
+      <c r="AE2" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="92" t="s">
+      <c r="AF2" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="95" t="s">
+      <c r="AG2" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="AH2" s="92" t="s">
+      <c r="AH2" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="AI2" s="92" t="s">
+      <c r="AI2" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="AJ2" s="93" t="s">
+      <c r="AJ2" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="93"/>
+      <c r="AK2" s="91"/>
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -17734,7 +17777,7 @@
       <c r="S3">
         <v>105.95673808436203</v>
       </c>
-      <c r="T3" s="98">
+      <c r="T3" s="96">
         <v>6.0286637702861946E-2</v>
       </c>
       <c r="U3">
@@ -17805,7 +17848,7 @@
       <c r="F4">
         <v>0.10428743961352656</v>
       </c>
-      <c r="G4" s="97">
+      <c r="G4" s="95">
         <v>6.3868296243536635</v>
       </c>
       <c r="H4">
@@ -17845,7 +17888,7 @@
       <c r="S4">
         <v>88.413855089759281</v>
       </c>
-      <c r="T4" s="98">
+      <c r="T4" s="96">
         <v>7.3966534094040193E-2</v>
       </c>
       <c r="U4">
@@ -17953,7 +17996,7 @@
       <c r="S5">
         <v>86.37003866174814</v>
       </c>
-      <c r="T5" s="99">
+      <c r="T5" s="97">
         <v>1.7679907819335386E-2</v>
       </c>
       <c r="U5">
@@ -18013,7 +18056,7 @@
         <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="E6">
         <v>0.16973888888888888</v>
@@ -18115,57 +18158,57 @@
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" t="s">
         <v>97</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>98</v>
-      </c>
-      <c r="D9" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" t="s">
         <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>